<commit_message>
adding in mark vs unmark comparison, more figures
</commit_message>
<xml_diff>
--- a/original_data/Net Mark Rate for Creel 2021-2023_021624_DateLineUpFINAL.xlsx
+++ b/original_data/Net Mark Rate for Creel 2021-2023_021624_DateLineUpFINAL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://stateofwa.sharepoint.com/sites/DFW-TeamFreshwaterCreelCo-ManagerWorkgroup/Shared Documents/General/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\NisquallyCreelInvestigation\original_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{BE06019F-19D8-4458-91FD-4EB13EFA5EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{979D46DA-E855-482C-BB54-1FD50D9D8CDC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F74958D5-FB19-4F70-A5C2-FDF749CAB5BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33840" yWindow="1500" windowWidth="30677" windowHeight="15103" activeTab="1" xr2:uid="{1063920B-2647-4EB3-92C1-83FBB13C6547}"/>
+    <workbookView xWindow="86280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1063920B-2647-4EB3-92C1-83FBB13C6547}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterate="1" iterateCount="10" iterateDelta="0.01"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId5"/>
     <pivotCache cacheId="1" r:id="rId6"/>
@@ -846,7 +846,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="129">
   <si>
     <t>New Method uses weekly GN Mark rate when available and Creel weekly when not</t>
   </si>
@@ -1227,6 +1227,12 @@
   </si>
   <si>
     <t xml:space="preserve">                                                                                                                          </t>
+  </si>
+  <si>
+    <t>ca</t>
+  </si>
+  <si>
+    <t>10/30-11/06</t>
   </si>
 </sst>
 </file>
@@ -3322,6 +3328,107 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2AB5E012-421B-4D94-9CF0-E79575B45ACF}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E2:F19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="2">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="17">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item x="14"/>
+        <item x="15"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="17">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Total Release" fld="1" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C54D3932-A25B-4DFB-B67E-5A031335A490}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O2:S19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
@@ -3430,107 +3537,6 @@
     <dataField name="Sum of Estimated CHUnK" fld="2" baseField="0" baseItem="0"/>
     <dataField name="Sum of Estimated CHMR" fld="3" baseField="0" baseItem="0"/>
     <dataField name="Sum of Estimated CHUnR" fld="4" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2AB5E012-421B-4D94-9CF0-E79575B45ACF}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="E2:F19" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="2">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="17">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-        <item x="14"/>
-        <item x="15"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="17">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
-    </i>
-    <i>
-      <x v="15"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Total Release" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -3843,25 +3849,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B3E7773-B67E-4CA8-8F67-6A56A7194F1E}">
   <dimension ref="A1:AI73"/>
   <sheetViews>
-    <sheetView zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView topLeftCell="C1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
+      <selection activeCell="W32" sqref="W32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3828125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.15234375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.53515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.3046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="26" width="12.53515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="11.15234375" customWidth="1"/>
-    <col min="30" max="30" width="12.53515625" customWidth="1"/>
-    <col min="31" max="31" width="16.15234375" customWidth="1"/>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="26" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.109375" customWidth="1"/>
+    <col min="30" max="30" width="12.5546875" customWidth="1"/>
+    <col min="31" max="31" width="16.109375" customWidth="1"/>
     <col min="32" max="35" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AC1" s="102"/>
       <c r="AD1" s="116" t="s">
         <v>0</v>
@@ -3872,7 +3878,7 @@
       <c r="AH1" s="116"/>
       <c r="AI1" s="117"/>
     </row>
-    <row r="2" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AC2" s="106"/>
       <c r="AD2" s="86" t="s">
         <v>1</v>
@@ -3893,7 +3899,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="124">
         <v>2021</v>
       </c>
@@ -3943,7 +3949,7 @@
         <v>584.88751318494121</v>
       </c>
     </row>
-    <row r="4" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="40"/>
       <c r="B4" s="122" t="s">
         <v>11</v>
@@ -4021,7 +4027,7 @@
         <v>0.37444010349988799</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
         <v>14</v>
       </c>
@@ -4108,7 +4114,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7" t="s">
         <v>18</v>
       </c>
@@ -4180,7 +4186,7 @@
         <v>1.0578852324150585</v>
       </c>
     </row>
-    <row r="7" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="7" t="s">
         <v>21</v>
       </c>
@@ -4263,7 +4269,7 @@
       <c r="AH7" s="122"/>
       <c r="AI7" s="22"/>
     </row>
-    <row r="8" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="7" t="s">
         <v>25</v>
       </c>
@@ -4364,7 +4370,7 @@
         <v>0.20103773390357327</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>29</v>
       </c>
@@ -4460,7 +4466,7 @@
       </c>
       <c r="AI9" s="104"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>33</v>
       </c>
@@ -4557,7 +4563,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
         <v>38</v>
       </c>
@@ -4654,7 +4660,7 @@
         <v>2.0104290565518813E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="7" t="s">
         <v>41</v>
       </c>
@@ -4740,7 +4746,7 @@
       </c>
       <c r="AI12" s="114"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
         <v>45</v>
       </c>
@@ -4806,7 +4812,7 @@
         <v>84.399593341976512</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>48</v>
       </c>
@@ -4872,7 +4878,7 @@
         <v>37.819072582304926</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>51</v>
       </c>
@@ -4946,7 +4952,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>54</v>
       </c>
@@ -5019,7 +5025,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="7" t="s">
         <v>58</v>
       </c>
@@ -5109,7 +5115,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>61</v>
       </c>
@@ -5198,7 +5204,7 @@
         <v>992.44184155149253</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>64</v>
       </c>
@@ -5286,7 +5292,7 @@
         <v>0.63535298239587701</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="10" t="s">
         <v>67</v>
       </c>
@@ -5368,7 +5374,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="J21" t="s">
         <v>70</v>
       </c>
@@ -5436,7 +5442,7 @@
         <v>0.3383061417819897</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
       <c r="U22" s="56">
         <f>U21/(U21+V21)</f>
         <v>0.70120293786363397</v>
@@ -5462,8 +5468,8 @@
         <v>0.37444010349988799</v>
       </c>
     </row>
-    <row r="23" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="24" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="24" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="L24" s="38"/>
       <c r="O24" s="60" t="s">
         <v>72</v>
@@ -5480,7 +5486,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O25" s="61"/>
       <c r="P25" s="62">
         <v>2021</v>
@@ -5529,7 +5535,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
       <c r="O26" s="64"/>
       <c r="P26" s="65"/>
       <c r="Q26" s="66"/>
@@ -5574,7 +5580,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
       <c r="O27" s="64">
         <v>26</v>
       </c>
@@ -5629,7 +5635,7 @@
         <v>0.16131687242798354</v>
       </c>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
       <c r="O28" s="64">
         <v>27</v>
       </c>
@@ -5658,7 +5664,7 @@
         <v>5.0438224763150581</v>
       </c>
     </row>
-    <row r="29" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O29" s="64">
         <v>28</v>
       </c>
@@ -5690,7 +5696,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O30" s="64">
         <v>29</v>
       </c>
@@ -5737,7 +5743,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
       <c r="O31" s="64">
         <v>30</v>
       </c>
@@ -5787,7 +5793,7 @@
         <v>349.06662561610057</v>
       </c>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
       <c r="O32" s="64">
         <v>31</v>
       </c>
@@ -5836,7 +5842,7 @@
         <v>0.22346953983050855</v>
       </c>
     </row>
-    <row r="33" spans="15:35" x14ac:dyDescent="0.4">
+    <row r="33" spans="15:35" x14ac:dyDescent="0.3">
       <c r="O33" s="64">
         <v>32</v>
       </c>
@@ -5885,7 +5891,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="15:35" x14ac:dyDescent="0.4">
+    <row r="34" spans="15:35" x14ac:dyDescent="0.3">
       <c r="O34" s="64">
         <v>33</v>
       </c>
@@ -5944,7 +5950,7 @@
         <v>0.12161088077508475</v>
       </c>
     </row>
-    <row r="35" spans="15:35" x14ac:dyDescent="0.4">
+    <row r="35" spans="15:35" x14ac:dyDescent="0.3">
       <c r="O35" s="64">
         <v>34</v>
       </c>
@@ -5979,7 +5985,7 @@
         <v>37.819072582304926</v>
       </c>
     </row>
-    <row r="36" spans="15:35" x14ac:dyDescent="0.4">
+    <row r="36" spans="15:35" x14ac:dyDescent="0.3">
       <c r="O36" s="64">
         <v>35</v>
       </c>
@@ -6014,7 +6020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O37" s="64">
         <v>36</v>
       </c>
@@ -6052,7 +6058,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O38" s="64">
         <v>37</v>
       </c>
@@ -6105,7 +6111,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="15:35" x14ac:dyDescent="0.4">
+    <row r="39" spans="15:35" x14ac:dyDescent="0.3">
       <c r="O39" s="64">
         <v>38</v>
       </c>
@@ -6161,7 +6167,7 @@
         <v>389.0815236864205</v>
       </c>
     </row>
-    <row r="40" spans="15:35" x14ac:dyDescent="0.4">
+    <row r="40" spans="15:35" x14ac:dyDescent="0.3">
       <c r="O40" s="64">
         <v>39</v>
       </c>
@@ -6214,7 +6220,7 @@
         <v>0.24908674354443094</v>
       </c>
     </row>
-    <row r="41" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O41" s="64">
         <v>40</v>
       </c>
@@ -6265,7 +6271,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O42" s="64">
         <v>41</v>
       </c>
@@ -6322,7 +6328,7 @@
         <v>0.1350883019855148</v>
       </c>
     </row>
-    <row r="43" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="O43" s="67">
         <v>42</v>
       </c>
@@ -6356,12 +6362,12 @@
         <v>0.63535298239587701</v>
       </c>
     </row>
-    <row r="44" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AE44" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="S45" s="43"/>
       <c r="T45" t="s">
         <v>79</v>
@@ -6387,7 +6393,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="15:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="S46" s="43"/>
       <c r="T46" s="1"/>
       <c r="U46" s="40" t="s">
@@ -6432,7 +6438,7 @@
         <v>765.43937940005856</v>
       </c>
     </row>
-    <row r="47" spans="15:35" x14ac:dyDescent="0.4">
+    <row r="47" spans="15:35" x14ac:dyDescent="0.3">
       <c r="S47" s="43"/>
       <c r="T47" s="7">
         <v>31</v>
@@ -6480,7 +6486,7 @@
         <v>0.4900279010655193</v>
       </c>
     </row>
-    <row r="48" spans="15:35" x14ac:dyDescent="0.4">
+    <row r="48" spans="15:35" x14ac:dyDescent="0.3">
       <c r="S48" s="43"/>
       <c r="T48" s="7">
         <v>32</v>
@@ -6528,7 +6534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="49" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S49" s="43"/>
       <c r="T49" s="7">
         <v>33</v>
@@ -6582,7 +6588,7 @@
         <v>0.26184942326572225</v>
       </c>
     </row>
-    <row r="50" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="50" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S50" s="43"/>
       <c r="T50" s="7">
         <v>34</v>
@@ -6612,7 +6618,7 @@
       <c r="AA50" s="43"/>
       <c r="AB50" s="43"/>
     </row>
-    <row r="51" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="51" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S51" s="43"/>
       <c r="T51" s="7">
         <v>35</v>
@@ -6642,7 +6648,7 @@
       <c r="AA51" s="43"/>
       <c r="AB51" s="43"/>
     </row>
-    <row r="52" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="52" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S52" s="43"/>
       <c r="T52" s="7">
         <v>36</v>
@@ -6672,7 +6678,7 @@
       <c r="AA52" s="43"/>
       <c r="AB52" s="43"/>
     </row>
-    <row r="53" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="53" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S53" s="43"/>
       <c r="T53" s="7">
         <v>37</v>
@@ -6702,7 +6708,7 @@
       <c r="AA53" s="43"/>
       <c r="AB53" s="43"/>
     </row>
-    <row r="54" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="54" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S54" s="43"/>
       <c r="T54" s="7">
         <v>38</v>
@@ -6732,7 +6738,7 @@
       <c r="AA54" s="43"/>
       <c r="AB54" s="43"/>
     </row>
-    <row r="55" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="55" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S55" s="43"/>
       <c r="T55" s="7">
         <v>39</v>
@@ -6762,7 +6768,7 @@
       <c r="AA55" s="43"/>
       <c r="AB55" s="43"/>
     </row>
-    <row r="56" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="56" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S56" s="43"/>
       <c r="T56" s="7">
         <v>40</v>
@@ -6792,7 +6798,7 @@
       <c r="AA56" s="43"/>
       <c r="AB56" s="43"/>
     </row>
-    <row r="57" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="57" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S57" s="43"/>
       <c r="T57" s="7">
         <v>41</v>
@@ -6822,7 +6828,7 @@
       <c r="AA57" s="43"/>
       <c r="AB57" s="43"/>
     </row>
-    <row r="58" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="58" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S58" s="43"/>
       <c r="T58" s="7">
         <v>42</v>
@@ -6852,7 +6858,7 @@
       <c r="AA58" s="43"/>
       <c r="AB58" s="43"/>
     </row>
-    <row r="59" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="59" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S59" s="43"/>
       <c r="T59" s="7">
         <v>43</v>
@@ -6882,7 +6888,7 @@
       <c r="AA59" s="43"/>
       <c r="AB59" s="43"/>
     </row>
-    <row r="60" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="60" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S60" s="43"/>
       <c r="T60" s="7">
         <v>44</v>
@@ -6912,7 +6918,7 @@
       <c r="AA60" s="43"/>
       <c r="AB60" s="43"/>
     </row>
-    <row r="61" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="61" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S61" s="43"/>
       <c r="T61" s="7">
         <v>45</v>
@@ -6942,7 +6948,7 @@
       <c r="AA61" s="43"/>
       <c r="AB61" s="43"/>
     </row>
-    <row r="62" spans="19:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="19:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="S62" s="43"/>
       <c r="T62" s="10">
         <v>46</v>
@@ -6972,7 +6978,7 @@
       <c r="AA62" s="43"/>
       <c r="AB62" s="43"/>
     </row>
-    <row r="63" spans="19:35" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="19:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="S63" s="43"/>
       <c r="T63" s="1" t="s">
         <v>71</v>
@@ -7003,7 +7009,7 @@
       </c>
       <c r="AA63" s="43"/>
     </row>
-    <row r="64" spans="19:35" x14ac:dyDescent="0.4">
+    <row r="64" spans="19:35" x14ac:dyDescent="0.3">
       <c r="S64" s="43"/>
       <c r="U64" s="56">
         <f>U63/(U63+V63)</f>
@@ -7031,7 +7037,7 @@
       </c>
       <c r="AA64" s="43"/>
     </row>
-    <row r="65" spans="19:28" x14ac:dyDescent="0.4">
+    <row r="65" spans="19:28" x14ac:dyDescent="0.3">
       <c r="S65" s="43"/>
       <c r="T65" s="43"/>
       <c r="U65" s="43"/>
@@ -7043,7 +7049,7 @@
       <c r="AA65" s="43"/>
       <c r="AB65" s="43"/>
     </row>
-    <row r="66" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="S66" s="43"/>
       <c r="T66" s="43" t="s">
         <v>80</v>
@@ -7057,7 +7063,7 @@
       <c r="AA66" s="43"/>
       <c r="AB66" s="43"/>
     </row>
-    <row r="67" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="T67" s="1" t="s">
         <v>71</v>
       </c>
@@ -7090,7 +7096,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="68" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="U68" s="75">
         <f>U67/(U67+V67)</f>
         <v>0.75091325645556906</v>
@@ -7123,12 +7129,12 @@
         <v>0.24908674354443094</v>
       </c>
     </row>
-    <row r="71" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="T71" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="72" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="T72" s="1" t="s">
         <v>71</v>
       </c>
@@ -7155,7 +7161,7 @@
         <v>765.43937940005856</v>
       </c>
     </row>
-    <row r="73" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="19:28" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="U73" s="75">
         <f>U72/(U72+V72)</f>
         <v>0.5099720989344807</v>
@@ -7196,34 +7202,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4D6E9B3-E44F-45EA-A765-6E49DAC03F9C}">
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="S26" sqref="S26"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.23046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.84375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.4609375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.69140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.69140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.84375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
         <v>2021</v>
@@ -7281,7 +7287,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="7">
         <v>31</v>
       </c>
@@ -7343,7 +7349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" s="7">
         <v>32</v>
       </c>
@@ -7405,7 +7411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" s="7">
         <v>33</v>
       </c>
@@ -7467,7 +7473,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" s="7">
         <v>34</v>
       </c>
@@ -7529,7 +7535,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>35</v>
       </c>
@@ -7591,7 +7597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="7">
         <v>36</v>
       </c>
@@ -7653,7 +7659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="7">
         <v>37</v>
       </c>
@@ -7715,7 +7721,7 @@
         <v>12.243102559685754</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="7">
         <v>38</v>
       </c>
@@ -7777,7 +7783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>39</v>
       </c>
@@ -7839,7 +7845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>40</v>
       </c>
@@ -7901,7 +7907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>41</v>
       </c>
@@ -7963,7 +7969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>42</v>
       </c>
@@ -8025,7 +8031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>43</v>
       </c>
@@ -8087,7 +8093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>44</v>
       </c>
@@ -8149,12 +8155,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>45</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="C16" s="7">
         <v>0</v>
@@ -8184,7 +8190,7 @@
         <v>45</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="O16" s="7">
         <v>0</v>
@@ -8211,7 +8217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
         <v>46</v>
       </c>
@@ -8273,7 +8279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>71</v>
       </c>
@@ -8335,7 +8341,7 @@
         <v>12.243102559685754</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="C19" s="56">
         <v>0.70120293786363397</v>
       </c>
@@ -8377,13 +8383,13 @@
         <v>0.37444010349988799</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G23" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.45"/>
-    <row r="25" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="1:22" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G25" s="1"/>
       <c r="H25" s="1">
         <v>2021</v>
@@ -8413,7 +8419,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G26" s="7">
         <v>31</v>
       </c>
@@ -8450,8 +8456,11 @@
         <f>SUM(J2,V2)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.4">
+      <c r="S26" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G27" s="7">
         <v>32</v>
       </c>
@@ -8489,7 +8498,7 @@
         <v>1.0578852324150585</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G28" s="7">
         <v>33</v>
       </c>
@@ -8527,7 +8536,7 @@
         <v>1.3360605952963525</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G29" s="7">
         <v>34</v>
       </c>
@@ -8565,7 +8574,7 @@
         <v>11.495952172148961</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G30" s="7">
         <v>35</v>
       </c>
@@ -8603,7 +8612,7 @@
         <v>19.050291163322768</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G31" s="7">
         <v>36</v>
       </c>
@@ -8641,7 +8650,7 @@
         <v>76.726378428367241</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="G32" s="7">
         <v>37</v>
       </c>
@@ -8679,7 +8688,7 @@
         <v>240.6329192470873</v>
       </c>
     </row>
-    <row r="33" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="33" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G33" s="7">
         <v>38</v>
       </c>
@@ -8717,7 +8726,7 @@
         <v>124.61246298170791</v>
       </c>
     </row>
-    <row r="34" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="34" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G34" s="7">
         <v>39</v>
       </c>
@@ -8755,7 +8764,7 @@
         <v>84.399593341976512</v>
       </c>
     </row>
-    <row r="35" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="35" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G35" s="7">
         <v>40</v>
       </c>
@@ -8793,7 +8802,7 @@
         <v>37.819072582304926</v>
       </c>
     </row>
-    <row r="36" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="36" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G36" s="7">
         <v>41</v>
       </c>
@@ -8831,7 +8840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="37" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G37" s="7">
         <v>42</v>
       </c>
@@ -8869,7 +8878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="38" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G38" s="7">
         <v>43</v>
       </c>
@@ -8907,7 +8916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="39" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G39" s="7">
         <v>44</v>
       </c>
@@ -8945,12 +8954,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="40" spans="7:18" x14ac:dyDescent="0.3">
       <c r="G40" s="7">
         <v>45</v>
       </c>
       <c r="H40" s="7" t="s">
-        <v>64</v>
+        <v>128</v>
       </c>
       <c r="I40" s="7">
         <f t="shared" si="0"/>
@@ -8983,7 +8992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="7:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="7:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G41" s="10">
         <v>46</v>
       </c>
@@ -9021,7 +9030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="7:18" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="7:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G42" s="1" t="s">
         <v>71</v>
       </c>
@@ -9053,7 +9062,7 @@
         <v>597.13061574462699</v>
       </c>
     </row>
-    <row r="43" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="43" spans="7:18" x14ac:dyDescent="0.3">
       <c r="I43" s="56">
         <v>0.70120293786363397</v>
       </c>
@@ -9075,7 +9084,7 @@
         <v>0.37444010349988799</v>
       </c>
     </row>
-    <row r="45" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="45" spans="7:18" x14ac:dyDescent="0.3">
       <c r="I45">
         <v>2021</v>
       </c>
@@ -9086,7 +9095,7 @@
         <v>2023</v>
       </c>
     </row>
-    <row r="46" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="46" spans="7:18" x14ac:dyDescent="0.3">
       <c r="H46" t="s">
         <v>97</v>
       </c>
@@ -9104,7 +9113,7 @@
         <v>11621.641406416058</v>
       </c>
     </row>
-    <row r="47" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="47" spans="7:18" x14ac:dyDescent="0.3">
       <c r="H47" t="s">
         <v>98</v>
       </c>
@@ -9122,7 +9131,7 @@
         <v>2235.5618174688834</v>
       </c>
     </row>
-    <row r="48" spans="7:18" x14ac:dyDescent="0.4">
+    <row r="48" spans="7:18" x14ac:dyDescent="0.3">
       <c r="I48" s="51"/>
       <c r="J48" s="138"/>
       <c r="L48" s="51"/>
@@ -9136,7 +9145,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="8:18" x14ac:dyDescent="0.4">
+    <row r="49" spans="8:18" x14ac:dyDescent="0.3">
       <c r="H49" t="s">
         <v>101</v>
       </c>
@@ -9161,7 +9170,7 @@
         <v>0.20863670127137979</v>
       </c>
     </row>
-    <row r="50" spans="8:18" x14ac:dyDescent="0.4">
+    <row r="50" spans="8:18" x14ac:dyDescent="0.3">
       <c r="H50" t="s">
         <v>102</v>
       </c>
@@ -9196,18 +9205,19 @@
   <dimension ref="A1:H107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="16.15234375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.53515625" style="8" customWidth="1"/>
-    <col min="4" max="5" width="14.53515625" style="38" customWidth="1"/>
-    <col min="6" max="6" width="23.84375" customWidth="1"/>
+    <col min="2" max="2" width="16.109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.5546875" style="8" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="38" customWidth="1"/>
+    <col min="5" max="5" width="21" style="38" customWidth="1"/>
+    <col min="6" max="6" width="23.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -9233,7 +9243,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>WEEKNUM(B2)</f>
         <v>32</v>
@@ -9261,7 +9271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <f t="shared" ref="A3:A66" si="0">WEEKNUM(B3)</f>
         <v>32</v>
@@ -9289,7 +9299,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -9317,7 +9327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -9345,7 +9355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -9373,7 +9383,7 @@
         <v>5.0264875103192983</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -9401,7 +9411,7 @@
         <v>2.5132437551596492</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -9429,7 +9439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -9457,7 +9467,7 @@
         <v>2.8288641224822539</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -9485,7 +9495,7 @@
         <v>2.8288641224822539</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -9513,7 +9523,7 @@
         <v>5.6577282449645079</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -9541,7 +9551,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -9569,7 +9579,7 @@
         <v>8.1637418784462934</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -9597,7 +9607,7 @@
         <v>11.332533979753741</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -9625,7 +9635,7 @@
         <v>9.7481379291000163</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -9653,7 +9663,7 @@
         <v>8.6620668851195042</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -9681,7 +9691,7 @@
         <v>12.700411988570272</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -9709,7 +9719,7 @@
         <v>10.681239436844887</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -9737,7 +9747,7 @@
         <v>10.681239436844887</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -9765,7 +9775,7 @@
         <v>73.12988723652245</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -9793,7 +9803,7 @@
         <v>79.507291614171322</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -9811,7 +9821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -9829,7 +9839,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -9857,7 +9867,7 @@
         <v>73.212251957634322</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -9885,7 +9895,7 @@
         <v>50.455456558362805</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -9913,7 +9923,7 @@
         <v>95.969047356905847</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -9941,7 +9951,7 @@
         <v>275.40973112787572</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -9969,7 +9979,7 @@
         <v>163.4067025588177</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -9987,7 +9997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -10005,7 +10015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -10033,7 +10043,7 @@
         <v>151.55528413399404</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -10061,7 +10071,7 @@
         <v>69.674787782918784</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -10089,7 +10099,7 @@
         <v>110.61503595845642</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -10117,7 +10127,7 @@
         <v>112.02003162559362</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -10145,7 +10155,7 @@
         <v>161.12222975479736</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -10163,7 +10173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -10181,7 +10191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -10209,7 +10219,7 @@
         <v>51.082167129874712</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -10237,7 +10247,7 @@
         <v>51.406946401757381</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -10265,7 +10275,7 @@
         <v>51.24455676581605</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -10293,7 +10303,7 @@
         <v>70.394528026291098</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -10321,7 +10331,7 @@
         <v>70.394528026291098</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -10349,7 +10359,7 @@
         <v>70.394528026291098</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -10377,7 +10387,7 @@
         <v>64.027063784717683</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -10405,7 +10415,7 @@
         <v>59.78516918644646</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -10433,7 +10443,7 @@
         <v>68.268958382988899</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -10461,7 +10471,7 @@
         <v>64.027063784717683</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -10489,7 +10499,7 @@
         <v>32.805995062592764</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -10517,7 +10527,7 @@
         <v>84.578217251824213</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -10545,7 +10555,7 @@
         <v>34.942287118716592</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -10573,7 +10583,7 @@
         <v>57.045168968026523</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -10601,7 +10611,7 @@
         <v>36.049756337944544</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -10629,7 +10639,7 @@
         <v>36.049756337944544</v>
       </c>
     </row>
-    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -10657,7 +10667,7 @@
         <v>15.054343707862568</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -10685,7 +10695,7 @@
         <v>19.86879432624113</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -10713,7 +10723,7 @@
         <v>31.286786291966777</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -10741,7 +10751,7 @@
         <v>42.704778257692425</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -10769,7 +10779,7 @@
         <v>35.312535828925299</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -10797,7 +10807,7 @@
         <v>69.208708959632517</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -10825,7 +10835,7 @@
         <v>35.312535828925299</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -10853,7 +10863,7 @@
         <v>1.4163626982180806</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -10881,7 +10891,7 @@
         <v>29.350265466514163</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -10909,7 +10919,7 @@
         <v>29.350265466514163</v>
       </c>
     </row>
-    <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -10927,7 +10937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -10945,7 +10955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -10973,7 +10983,7 @@
         <v>2.9447681168073028</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <f t="shared" ref="A67:A107" si="2">WEEKNUM(B67)</f>
         <v>41</v>
@@ -11001,7 +11011,7 @@
         <v>1.4723840584036514</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -11029,7 +11039,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -11057,7 +11067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <f t="shared" si="2"/>
         <v>41</v>
@@ -11085,7 +11095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -11103,7 +11113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A72">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -11121,7 +11131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A73">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -11149,7 +11159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A74">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -11177,7 +11187,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -11205,7 +11215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A76">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -11233,7 +11243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A77">
         <f t="shared" si="2"/>
         <v>42</v>
@@ -11261,7 +11271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A78">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -11279,7 +11289,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A79">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -11297,7 +11307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A80">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -11325,7 +11335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A81">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -11353,7 +11363,7 @@
         <v>0.38081649831649822</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A82">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -11381,7 +11391,7 @@
         <v>0.69040824915824905</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A83">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -11409,7 +11419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A84">
         <f t="shared" si="2"/>
         <v>43</v>
@@ -11437,7 +11447,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A85">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -11455,7 +11465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A86">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -11473,7 +11483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A87">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -11501,7 +11511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A88">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -11529,7 +11539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A89">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -11557,7 +11567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A90">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -11585,7 +11595,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A91">
         <f t="shared" si="2"/>
         <v>44</v>
@@ -11613,7 +11623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A92">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -11631,7 +11641,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A93">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -11649,7 +11659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A94">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -11677,7 +11687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A95">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -11705,7 +11715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A96">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -11733,7 +11743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A97">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -11761,7 +11771,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A98">
         <f t="shared" si="2"/>
         <v>45</v>
@@ -11789,7 +11799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A99">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -11807,7 +11817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A100">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -11825,7 +11835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A101">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -11853,7 +11863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A102">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -11881,7 +11891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A103">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -11909,7 +11919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -11937,7 +11947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A105">
         <f t="shared" si="2"/>
         <v>46</v>
@@ -11965,7 +11975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A106">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -11983,7 +11993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A107">
         <f t="shared" si="2"/>
         <v>47</v>
@@ -12011,26 +12021,26 @@
   <dimension ref="A1:AA107"/>
   <sheetViews>
     <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AA4" sqref="AA4"/>
+      <selection activeCell="W18" sqref="W18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.84375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="14.53515625" style="38" customWidth="1"/>
-    <col min="15" max="15" width="12.69140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.69140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="22.3046875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.69140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="22.3046875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.69140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="22.3046875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="21.69140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.3046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.5546875" style="38" customWidth="1"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>103</v>
       </c>
@@ -12056,7 +12066,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>32</v>
       </c>
@@ -12115,7 +12125,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>32</v>
       </c>
@@ -12181,7 +12191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>32</v>
       </c>
@@ -12247,7 +12257,7 @@
         <v>0.83177804578305292</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>32</v>
       </c>
@@ -12313,7 +12323,7 @@
         <v>0.56467380803511835</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>32</v>
       </c>
@@ -12379,7 +12389,7 @@
         <v>0.64676912994183966</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>32</v>
       </c>
@@ -12445,7 +12455,7 @@
         <v>0.51288082768197352</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>33</v>
       </c>
@@ -12511,7 +12521,7 @@
         <v>0.67358168614753655</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>33</v>
       </c>
@@ -12577,7 +12587,7 @@
         <v>0.66432747805812487</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>33</v>
       </c>
@@ -12643,7 +12653,7 @@
         <v>0.70397979388317533</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>33</v>
       </c>
@@ -12709,7 +12719,7 @@
         <v>0.92609565616235567</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>33</v>
       </c>
@@ -12775,7 +12785,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>33</v>
       </c>
@@ -12841,7 +12851,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>33</v>
       </c>
@@ -12907,7 +12917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>34</v>
       </c>
@@ -12973,7 +12983,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>34</v>
       </c>
@@ -13039,7 +13049,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>34</v>
       </c>
@@ -13105,7 +13115,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>34</v>
       </c>
@@ -13151,7 +13161,7 @@
       <c r="X18" s="33"/>
       <c r="Y18" s="33"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>34</v>
       </c>
@@ -13198,7 +13208,7 @@
         <v>1790.8813841599342</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>34</v>
       </c>
@@ -13224,7 +13234,7 @@
         <v>73.12988723652245</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>34</v>
       </c>
@@ -13250,7 +13260,7 @@
         <v>79.507291614171322</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>35</v>
       </c>
@@ -13266,7 +13276,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>35</v>
       </c>
@@ -13282,7 +13292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>35</v>
       </c>
@@ -13308,7 +13318,7 @@
         <v>73.212251957634322</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>35</v>
       </c>
@@ -13334,7 +13344,7 @@
         <v>50.455456558362805</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>35</v>
       </c>
@@ -13360,7 +13370,7 @@
         <v>95.969047356905847</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>35</v>
       </c>
@@ -13386,7 +13396,7 @@
         <v>275.40973112787572</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>35</v>
       </c>
@@ -13412,7 +13422,7 @@
         <v>163.4067025588177</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>36</v>
       </c>
@@ -13428,7 +13438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>36</v>
       </c>
@@ -13444,7 +13454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>36</v>
       </c>
@@ -13470,7 +13480,7 @@
         <v>151.55528413399404</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>36</v>
       </c>
@@ -13496,7 +13506,7 @@
         <v>69.674787782918784</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>36</v>
       </c>
@@ -13522,7 +13532,7 @@
         <v>110.61503595845642</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>36</v>
       </c>
@@ -13548,7 +13558,7 @@
         <v>112.02003162559362</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>36</v>
       </c>
@@ -13574,7 +13584,7 @@
         <v>161.12222975479736</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>37</v>
       </c>
@@ -13590,7 +13600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>37</v>
       </c>
@@ -13606,7 +13616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -13632,7 +13642,7 @@
         <v>51.082167129874712</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>37</v>
       </c>
@@ -13658,7 +13668,7 @@
         <v>51.406946401757381</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>37</v>
       </c>
@@ -13684,7 +13694,7 @@
         <v>51.24455676581605</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>37</v>
       </c>
@@ -13710,7 +13720,7 @@
         <v>70.394528026291098</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>37</v>
       </c>
@@ -13736,7 +13746,7 @@
         <v>70.394528026291098</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>38</v>
       </c>
@@ -13762,7 +13772,7 @@
         <v>70.394528026291098</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>38</v>
       </c>
@@ -13788,7 +13798,7 @@
         <v>64.027063784717683</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>38</v>
       </c>
@@ -13814,7 +13824,7 @@
         <v>59.78516918644646</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>38</v>
       </c>
@@ -13840,7 +13850,7 @@
         <v>68.268958382988899</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>38</v>
       </c>
@@ -13866,7 +13876,7 @@
         <v>64.027063784717683</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>38</v>
       </c>
@@ -13892,7 +13902,7 @@
         <v>32.805995062592764</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>38</v>
       </c>
@@ -13918,7 +13928,7 @@
         <v>84.578217251824213</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>39</v>
       </c>
@@ -13944,7 +13954,7 @@
         <v>34.942287118716592</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>39</v>
       </c>
@@ -13970,7 +13980,7 @@
         <v>57.045168968026523</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>39</v>
       </c>
@@ -13996,7 +14006,7 @@
         <v>36.049756337944544</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>39</v>
       </c>
@@ -14022,7 +14032,7 @@
         <v>36.049756337944544</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>39</v>
       </c>
@@ -14048,7 +14058,7 @@
         <v>15.054343707862568</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>39</v>
       </c>
@@ -14074,7 +14084,7 @@
         <v>19.86879432624113</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>39</v>
       </c>
@@ -14100,7 +14110,7 @@
         <v>31.286786291966777</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>40</v>
       </c>
@@ -14126,7 +14136,7 @@
         <v>42.704778257692425</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>40</v>
       </c>
@@ -14152,7 +14162,7 @@
         <v>35.312535828925299</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>40</v>
       </c>
@@ -14178,7 +14188,7 @@
         <v>69.208708959632517</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>40</v>
       </c>
@@ -14204,7 +14214,7 @@
         <v>35.312535828925299</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>40</v>
       </c>
@@ -14230,7 +14240,7 @@
         <v>1.4163626982180806</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>40</v>
       </c>
@@ -14256,7 +14266,7 @@
         <v>29.350265466514163</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>40</v>
       </c>
@@ -14282,7 +14292,7 @@
         <v>29.350265466514163</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>41</v>
       </c>
@@ -14298,7 +14308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>41</v>
       </c>
@@ -14314,7 +14324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>41</v>
       </c>
@@ -14340,7 +14350,7 @@
         <v>2.9447681168073028</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>41</v>
       </c>
@@ -14366,7 +14376,7 @@
         <v>1.4723840584036514</v>
       </c>
     </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>41</v>
       </c>
@@ -14392,7 +14402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>41</v>
       </c>
@@ -14418,7 +14428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>41</v>
       </c>
@@ -14444,7 +14454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>42</v>
       </c>
@@ -14460,7 +14470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>42</v>
       </c>
@@ -14476,7 +14486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>42</v>
       </c>
@@ -14502,7 +14512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>42</v>
       </c>
@@ -14528,7 +14538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>42</v>
       </c>
@@ -14554,7 +14564,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>42</v>
       </c>
@@ -14580,7 +14590,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>42</v>
       </c>
@@ -14606,7 +14616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>43</v>
       </c>
@@ -14622,7 +14632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>43</v>
       </c>
@@ -14638,7 +14648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>43</v>
       </c>
@@ -14664,7 +14674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>43</v>
       </c>
@@ -14690,7 +14700,7 @@
         <v>0.38081649831649822</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>43</v>
       </c>
@@ -14716,7 +14726,7 @@
         <v>0.69040824915824905</v>
       </c>
     </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>43</v>
       </c>
@@ -14742,7 +14752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>43</v>
       </c>
@@ -14768,7 +14778,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>44</v>
       </c>
@@ -14784,7 +14794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>44</v>
       </c>
@@ -14800,7 +14810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>44</v>
       </c>
@@ -14826,7 +14836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>44</v>
       </c>
@@ -14852,7 +14862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>44</v>
       </c>
@@ -14878,7 +14888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>44</v>
       </c>
@@ -14904,7 +14914,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>44</v>
       </c>
@@ -14930,7 +14940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>45</v>
       </c>
@@ -14946,7 +14956,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>45</v>
       </c>
@@ -14962,7 +14972,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>45</v>
       </c>
@@ -14988,7 +14998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>45</v>
       </c>
@@ -15014,7 +15024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>45</v>
       </c>
@@ -15040,7 +15050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>45</v>
       </c>
@@ -15066,7 +15076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>45</v>
       </c>
@@ -15092,7 +15102,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>46</v>
       </c>
@@ -15108,7 +15118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>46</v>
       </c>
@@ -15124,7 +15134,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>46</v>
       </c>
@@ -15150,7 +15160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102">
         <v>46</v>
       </c>
@@ -15176,7 +15186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103">
         <v>46</v>
       </c>
@@ -15202,7 +15212,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104">
         <v>46</v>
       </c>
@@ -15228,7 +15238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105">
         <v>46</v>
       </c>
@@ -15254,7 +15264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106">
         <v>47</v>
       </c>
@@ -15270,7 +15280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107">
         <v>47</v>
       </c>
@@ -15292,6 +15302,24 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010019DB00D99CB47747BF3A0DACBFC204A4" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb31d097d37c8b713b7587c289c1c32b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="560ee0e8-f1f0-4f63-b31e-504d3324d09a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="eb178252b4395c83472c856a34907d29" ns1:_="" ns2:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -15452,25 +15480,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C092A0A2-7D77-4C92-B330-118F0C23C81F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76755908-904B-4783-AE1E-1DC06F0C6521}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17C75AD3-62E7-4BA8-8950-FA0AFE726EB1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -15487,22 +15515,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76755908-904B-4783-AE1E-1DC06F0C6521}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C092A0A2-7D77-4C92-B330-118F0C23C81F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>